<commit_message>
Data Analysis v0.7 develop
</commit_message>
<xml_diff>
--- a/example/test_coverage_new_example.xlsx
+++ b/example/test_coverage_new_example.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2F24B2-3B84-4F88-BC3A-3506000D04B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44A139E-FA74-4040-9CD9-A9788DD14705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="2610" windowWidth="21600" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="285" yWindow="3570" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -463,7 +463,7 @@
         <v>0.45761368873757857</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D2">
         <v>0.85182854920744511</v>
@@ -548,7 +548,7 @@
         <v>0.29059591908711324</v>
       </c>
       <c r="C7">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="D7">
         <v>0.13711387802753638</v>
@@ -616,7 +616,7 @@
         <v>0.9806942805560489</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D11">
         <v>0.50391598447905039</v>
@@ -667,7 +667,7 @@
         <v>0.71662015702671911</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D14">
         <v>0.56992175026882408</v>

</xml_diff>